<commit_message>
[PdP] - Corretto errore.
</commit_message>
<xml_diff>
--- a/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbazzerl/Desktop/SWE/Monolith GitHub/GANTT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbazzerl/Desktop/SWE/Monolith GitHub/documenti/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30785,8 +30785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[PdP] - Modificata anche sezione Consuntivo. Mancano solo da aggiungere le ore e i costi al termine del periodo in corso.
</commit_message>
<xml_diff>
--- a/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ARM" sheetId="1" r:id="rId1"/>
@@ -256,19 +256,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -823,11 +823,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2143034080"/>
-        <c:axId val="2143037632"/>
+        <c:axId val="-2147199008"/>
+        <c:axId val="-2147202560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143034080"/>
+        <c:axId val="-2147199008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +870,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143037632"/>
+        <c:crossAx val="-2147202560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -878,7 +878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143037632"/>
+        <c:axId val="-2147202560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +929,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143034080"/>
+        <c:crossAx val="-2147199008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,7 +943,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1215,9 +1214,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1287,9 +1284,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1372,7 +1367,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1977,11 +1971,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2143456768"/>
-        <c:axId val="2143460304"/>
+        <c:axId val="2123254896"/>
+        <c:axId val="2123258432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143456768"/>
+        <c:axId val="2123254896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +2018,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143460304"/>
+        <c:crossAx val="2123258432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2032,7 +2026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143460304"/>
+        <c:axId val="2123258432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2077,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143456768"/>
+        <c:crossAx val="2123254896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2097,7 +2091,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2378,9 +2371,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2450,9 +2441,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2535,7 +2524,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2810,9 +2798,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2882,9 +2868,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2967,7 +2951,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -3572,11 +3555,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2143592656"/>
-        <c:axId val="2143596192"/>
+        <c:axId val="-2147378912"/>
+        <c:axId val="-2147382464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143592656"/>
+        <c:axId val="-2147378912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3619,7 +3602,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143596192"/>
+        <c:crossAx val="-2147382464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3627,7 +3610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143596192"/>
+        <c:axId val="-2147382464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3678,7 +3661,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143592656"/>
+        <c:crossAx val="-2147378912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4013,9 +3996,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4034,9 +4015,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4055,9 +4034,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4127,9 +4104,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4222,7 +4197,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -4535,9 +4509,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4556,9 +4528,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4628,9 +4598,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4723,7 +4691,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5328,11 +5295,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2094598368"/>
-        <c:axId val="-2101384144"/>
+        <c:axId val="-2144807616"/>
+        <c:axId val="-2144804064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2094598368"/>
+        <c:axId val="-2144807616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5375,7 +5342,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101384144"/>
+        <c:crossAx val="-2144804064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5383,7 +5350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101384144"/>
+        <c:axId val="-2144804064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5434,7 +5401,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094598368"/>
+        <c:crossAx val="-2144807616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5748,9 +5715,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5820,9 +5785,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5915,7 +5878,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6218,9 +6180,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6290,9 +6250,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6385,7 +6343,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6722,9 +6679,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6807,7 +6762,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -7412,11 +7366,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2142217248"/>
-        <c:axId val="2142220784"/>
+        <c:axId val="-2144684960"/>
+        <c:axId val="-2144681424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142217248"/>
+        <c:axId val="-2144684960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7459,7 +7413,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142220784"/>
+        <c:crossAx val="-2144681424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7467,7 +7421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142220784"/>
+        <c:axId val="-2144681424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7518,7 +7472,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142217248"/>
+        <c:crossAx val="-2144684960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7532,7 +7486,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7853,9 +7806,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7925,9 +7876,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -8020,7 +7969,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -8321,7 +8269,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8345,7 +8292,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8353,7 +8299,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8377,7 +8322,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8385,7 +8329,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8409,7 +8352,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8417,7 +8359,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8441,7 +8382,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8662,7 +8602,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -9015,9 +8954,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9036,9 +8973,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9057,9 +8992,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9078,9 +9011,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9099,9 +9030,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9171,9 +9100,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9276,7 +9203,6 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -9629,9 +9555,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9650,9 +9574,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9671,9 +9593,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9743,9 +9663,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9848,7 +9766,6 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -10453,11 +10370,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2144587488"/>
-        <c:axId val="2144591056"/>
+        <c:axId val="-2144485888"/>
+        <c:axId val="-2144482320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144587488"/>
+        <c:axId val="-2144485888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10500,7 +10417,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144591056"/>
+        <c:crossAx val="-2144482320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10508,7 +10425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144591056"/>
+        <c:axId val="-2144482320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10559,7 +10476,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144587488"/>
+        <c:crossAx val="-2144485888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10573,7 +10490,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10938,9 +10854,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11031,7 +10945,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -11695,11 +11608,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2142019376"/>
-        <c:axId val="2142022912"/>
+        <c:axId val="-2146368752"/>
+        <c:axId val="-2146372304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142019376"/>
+        <c:axId val="-2146368752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11742,7 +11655,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142022912"/>
+        <c:crossAx val="-2146372304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11750,7 +11663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142022912"/>
+        <c:axId val="-2146372304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11801,7 +11714,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142019376"/>
+        <c:crossAx val="-2146368752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12137,11 +12050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="2143202256"/>
-        <c:axId val="2143205664"/>
+        <c:axId val="2123444112"/>
+        <c:axId val="2123440464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143202256"/>
+        <c:axId val="2123444112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12179,7 +12092,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143205664"/>
+        <c:crossAx val="2123440464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12187,7 +12100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143205664"/>
+        <c:axId val="2123440464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12250,7 +12163,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143202256"/>
+        <c:crossAx val="2123444112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12828,11 +12741,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2140454096"/>
-        <c:axId val="2140457632"/>
+        <c:axId val="-2145019184"/>
+        <c:axId val="-2145015648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140454096"/>
+        <c:axId val="-2145019184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12875,7 +12788,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140457632"/>
+        <c:crossAx val="-2145015648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12883,7 +12796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140457632"/>
+        <c:axId val="-2145015648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12934,7 +12847,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140454096"/>
+        <c:crossAx val="-2145019184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12948,7 +12861,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13282,9 +13194,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -13367,7 +13277,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -13972,11 +13881,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2143258352"/>
-        <c:axId val="2143261888"/>
+        <c:axId val="2123471856"/>
+        <c:axId val="2123435056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143258352"/>
+        <c:axId val="2123471856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14019,7 +13928,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143261888"/>
+        <c:crossAx val="2123435056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14027,7 +13936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143261888"/>
+        <c:axId val="2123435056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14078,7 +13987,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143258352"/>
+        <c:crossAx val="2123471856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14092,7 +14001,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14375,9 +14283,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -14447,9 +14353,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -14532,7 +14436,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -31806,52 +31709,52 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="8">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="8">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="8">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
@@ -31859,81 +31762,81 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="8">
         <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="7"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="8"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="8">
         <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="7"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="8"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B87" s="8">
         <v>750</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="8"/>
-      <c r="B88" s="7"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="8"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="8">
         <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="7"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="8"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="9"/>
-      <c r="B91" s="7"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="8"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="9"/>
-      <c r="B92" s="7"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A91:A92"/>
     <mergeCell ref="B91:B92"/>
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="B87:B88"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32256,52 +32159,52 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="8">
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -32578,103 +32481,111 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="8">
         <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="8">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="8">
         <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="8"/>
-      <c r="B81" s="7"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="8"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="7">
+      <c r="B82" s="8">
         <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
-      <c r="B83" s="7"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="8"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84" s="8">
         <v>2640</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8"/>
-      <c r="B85" s="7"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="8"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86" s="8">
         <v>975</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="7"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="B84:B85"/>
     <mergeCell ref="A86:A87"/>
@@ -32683,14 +32594,6 @@
     <mergeCell ref="B80:B81"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32956,103 +32859,111 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="8">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="8">
         <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86" s="8">
         <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="7"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="8"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B88" s="8">
         <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="8"/>
-      <c r="B89" s="7"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="8"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B90" s="7">
+      <c r="B90" s="8">
         <v>1430</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="8"/>
-      <c r="B91" s="7"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="8"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B92" s="8">
         <v>630</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="8"/>
-      <c r="B93" s="7"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A90:A91"/>
     <mergeCell ref="B90:B91"/>
     <mergeCell ref="A92:A93"/>
@@ -33061,14 +32972,6 @@
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B88:B89"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33079,7 +32982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="135" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="135" workbookViewId="0">
       <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
@@ -33347,174 +33250,160 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="8">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="8">
         <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="8">
         <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="8">
         <v>330</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="8"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79" s="8">
         <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="7"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="8"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81" s="8">
         <v>462</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="7"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="8"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="8">
         <v>2055</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="7"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="8"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="8">
         <f>1155</f>
         <v>1155</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="7"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="8"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="7">
+      <c r="B97" s="8">
         <v>210</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="7"/>
+      <c r="B98" s="8"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="7">
+      <c r="B99" s="8">
         <v>140</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="7"/>
+      <c r="B100" s="8"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="7">
+      <c r="B101" s="8">
         <v>1430</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="7"/>
+      <c r="B102" s="8"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="7">
+      <c r="B103" s="8">
         <v>630</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="7"/>
+      <c r="B104" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A51:A52"/>
@@ -33525,6 +33414,20 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33535,7 +33438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A2" zoomScale="150" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -33795,127 +33698,139 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="8">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="8">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="8">
         <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="8">
         <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="8">
         <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="8">
         <v>540</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="8">
         <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="8">
         <v>1892</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="8"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="8">
         <v>2055</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="8"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="8">
         <v>1785</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -33924,18 +33839,6 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -34258,55 +34161,55 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
-      <c r="B45" s="7"/>
+      <c r="B45" s="8"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B46" s="11">
@@ -34314,55 +34217,55 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
+      <c r="A47" s="8"/>
       <c r="B47" s="11"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="7">
+      <c r="B75" s="8">
         <v>420</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
+      <c r="B76" s="8"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="8">
         <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="8"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79" s="8">
         <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="7"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="8"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81" s="8">
         <v>1035</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="7"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="8"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B83" s="11">
@@ -34370,7 +34273,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
+      <c r="A84" s="9"/>
       <c r="B84" s="11"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -34383,12 +34286,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B83:B84"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -34399,6 +34296,12 @@
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B83:B84"/>
     <mergeCell ref="A81:A82"/>
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="A83:A84"/>
@@ -34421,148 +34324,148 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
         <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="8">
         <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="8">
         <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="8">
         <v>1230</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="8">
         <v>620</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="8">
         <v>750</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="8">
         <v>4796</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="8">
         <v>2220</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="8">
         <v>4005</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -34749,39 +34652,39 @@
       </c>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F94" s="16" t="s">
+      <c r="F94" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G94" s="16" t="s">
+      <c r="G94" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H94" s="16" t="s">
+      <c r="H94" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I94" s="16" t="s">
+      <c r="I94" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J94" s="16" t="s">
+      <c r="J94" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K94" s="16" t="s">
+      <c r="K94" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E95" s="16"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
-      <c r="J95" s="16"/>
-      <c r="K95" s="16"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
     </row>
     <row r="96" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E96" s="17" t="s">
+      <c r="E96" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F96" s="14">
@@ -34804,7 +34707,7 @@
       </c>
     </row>
     <row r="97" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E97" s="17"/>
+      <c r="E97" s="16"/>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
@@ -34813,7 +34716,7 @@
       <c r="K97" s="14"/>
     </row>
     <row r="98" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E98" s="15" t="s">
+      <c r="E98" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F98" s="14">
@@ -34836,7 +34739,7 @@
       </c>
     </row>
     <row r="99" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E99" s="15"/>
+      <c r="E99" s="17"/>
       <c r="F99" s="14"/>
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
@@ -34845,7 +34748,7 @@
       <c r="K99" s="14"/>
     </row>
     <row r="100" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E100" s="15" t="s">
+      <c r="E100" s="17" t="s">
         <v>25</v>
       </c>
       <c r="F100" s="14">
@@ -34868,7 +34771,7 @@
       </c>
     </row>
     <row r="101" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E101" s="15"/>
+      <c r="E101" s="17"/>
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
@@ -34877,7 +34780,7 @@
       <c r="K101" s="14"/>
     </row>
     <row r="102" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E102" s="15" t="s">
+      <c r="E102" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F102" s="14">
@@ -34900,7 +34803,7 @@
       </c>
     </row>
     <row r="103" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E103" s="15"/>
+      <c r="E103" s="17"/>
       <c r="F103" s="14"/>
       <c r="G103" s="14"/>
       <c r="H103" s="14"/>
@@ -34909,7 +34812,7 @@
       <c r="K103" s="14"/>
     </row>
     <row r="104" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E104" s="15" t="s">
+      <c r="E104" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F104" s="14">
@@ -34932,7 +34835,7 @@
       </c>
     </row>
     <row r="105" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E105" s="15"/>
+      <c r="E105" s="17"/>
       <c r="F105" s="14"/>
       <c r="G105" s="14"/>
       <c r="H105" s="14"/>
@@ -34941,7 +34844,7 @@
       <c r="K105" s="14"/>
     </row>
     <row r="106" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E106" s="15" t="s">
+      <c r="E106" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F106" s="14">
@@ -34964,7 +34867,7 @@
       </c>
     </row>
     <row r="107" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E107" s="15"/>
+      <c r="E107" s="17"/>
       <c r="F107" s="14"/>
       <c r="G107" s="14"/>
       <c r="H107" s="14"/>
@@ -34973,7 +34876,7 @@
       <c r="K107" s="14"/>
     </row>
     <row r="108" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E108" s="15" t="s">
+      <c r="E108" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F108" s="14">
@@ -34996,7 +34899,7 @@
       </c>
     </row>
     <row r="109" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E109" s="15"/>
+      <c r="E109" s="17"/>
       <c r="F109" s="14"/>
       <c r="G109" s="14"/>
       <c r="H109" s="14"/>
@@ -35006,30 +34909,48 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="J102:J103"/>
+    <mergeCell ref="K102:K103"/>
+    <mergeCell ref="J100:J101"/>
+    <mergeCell ref="K100:K101"/>
+    <mergeCell ref="J98:J99"/>
+    <mergeCell ref="K98:K99"/>
+    <mergeCell ref="J108:J109"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="J106:J107"/>
+    <mergeCell ref="K106:K107"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="K104:K105"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="I108:I109"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="G106:G107"/>
+    <mergeCell ref="H106:H107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="G102:G103"/>
+    <mergeCell ref="H102:H103"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="G100:G101"/>
+    <mergeCell ref="H100:H101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="G98:G99"/>
+    <mergeCell ref="H98:H99"/>
+    <mergeCell ref="I98:I99"/>
     <mergeCell ref="J96:J97"/>
     <mergeCell ref="K96:K97"/>
     <mergeCell ref="H94:H95"/>
@@ -35044,48 +34965,30 @@
     <mergeCell ref="J94:J95"/>
     <mergeCell ref="K94:K95"/>
     <mergeCell ref="I96:I97"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="G98:G99"/>
-    <mergeCell ref="H98:H99"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="G100:G101"/>
-    <mergeCell ref="H100:H101"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="F102:F103"/>
-    <mergeCell ref="G102:G103"/>
-    <mergeCell ref="H102:H103"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="H104:H105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="G106:G107"/>
-    <mergeCell ref="H106:H107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="I108:I109"/>
-    <mergeCell ref="J108:J109"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="J106:J107"/>
-    <mergeCell ref="K106:K107"/>
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="K104:K105"/>
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="K102:K103"/>
-    <mergeCell ref="J100:J101"/>
-    <mergeCell ref="K100:K101"/>
-    <mergeCell ref="J98:J99"/>
-    <mergeCell ref="K98:K99"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[PdP] - Modificato piano di progetto. Aggiunte ore di autoapprendimento a periodo PDCOD. Aggiornata analisi dei rischi. Aggiunti relativi dati alle tabelle. Modificate relative immagini. Modificati Gantt e pianificazione. In attesa di verifica. TODO: Consuntivo di periodo.
</commit_message>
<xml_diff>
--- a/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbazzerl/Desktop/SWE/Monolith GitHub/documenti/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbazzerl/Desktop/SWE/MonolithGitHub/documenti/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ARM" sheetId="1" r:id="rId1"/>
@@ -256,19 +256,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -823,11 +823,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2147199008"/>
-        <c:axId val="-2147202560"/>
+        <c:axId val="2134747456"/>
+        <c:axId val="2134751008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2147199008"/>
+        <c:axId val="2134747456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +870,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2147202560"/>
+        <c:crossAx val="2134751008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -878,7 +878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2147202560"/>
+        <c:axId val="2134751008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +929,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2147199008"/>
+        <c:crossAx val="2134747456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,6 +943,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1971,11 +1972,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2123254896"/>
-        <c:axId val="2123258432"/>
+        <c:axId val="2104320208"/>
+        <c:axId val="2104323744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123254896"/>
+        <c:axId val="2104320208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,7 +2019,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123258432"/>
+        <c:crossAx val="2104323744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2026,7 +2027,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123258432"/>
+        <c:axId val="2104323744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2077,7 +2078,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123254896"/>
+        <c:crossAx val="2104320208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2091,6 +2092,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3437,25 +3439,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>22.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.0</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3521,25 +3523,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3555,11 +3557,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2147378912"/>
-        <c:axId val="-2147382464"/>
+        <c:axId val="2136063280"/>
+        <c:axId val="2136066816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2147378912"/>
+        <c:axId val="2136063280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3602,7 +3604,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2147382464"/>
+        <c:crossAx val="2136066816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3610,7 +3612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2147382464"/>
+        <c:axId val="2136066816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3661,7 +3663,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2147378912"/>
+        <c:crossAx val="2136063280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3996,7 +3998,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4015,7 +4019,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4034,7 +4040,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4104,7 +4112,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4146,10 +4156,10 @@
                   <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137.0</c:v>
+                  <c:v>193.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.0</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4197,6 +4207,7 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -4509,7 +4520,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4528,7 +4541,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4598,7 +4613,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4691,6 +4708,7 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5177,25 +5195,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>22.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.0</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5261,25 +5279,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5295,11 +5313,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2144807616"/>
-        <c:axId val="-2144804064"/>
+        <c:axId val="2104420048"/>
+        <c:axId val="2104423584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144807616"/>
+        <c:axId val="2104420048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5342,7 +5360,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144804064"/>
+        <c:crossAx val="2104423584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5350,7 +5368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144804064"/>
+        <c:axId val="2104423584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5401,7 +5419,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144807616"/>
+        <c:crossAx val="2104420048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5715,7 +5733,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5785,7 +5805,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5827,10 +5849,10 @@
                   <c:v>86.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137.0</c:v>
+                  <c:v>193.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119.0</c:v>
+                  <c:v>133.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5878,6 +5900,7 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6180,7 +6203,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6250,7 +6275,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6343,6 +6370,7 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6679,7 +6707,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6762,6 +6792,7 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -7366,11 +7397,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2144684960"/>
-        <c:axId val="-2144681424"/>
+        <c:axId val="2104452928"/>
+        <c:axId val="2104456464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144684960"/>
+        <c:axId val="2104452928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7413,7 +7444,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144681424"/>
+        <c:crossAx val="2104456464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7421,7 +7452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144681424"/>
+        <c:axId val="2104456464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7472,7 +7503,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144684960"/>
+        <c:crossAx val="2104452928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8269,13 +8300,14 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
                     <a:fld id="{A6D8E32A-ABD1-EB42-B8EF-5D102E5643CA}" type="PERCENTAGE">
-                      <a:rPr lang="is-IS" sz="2000"/>
+                      <a:rPr lang="mr-IN" sz="2000"/>
                       <a:pPr/>
                       <a:t>[PERCENTUALE]</a:t>
                     </a:fld>
@@ -8292,6 +8324,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8299,13 +8332,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
                     <a:fld id="{E152E207-B13B-6642-BAB1-CD571DF6F864}" type="PERCENTAGE">
-                      <a:rPr lang="pt-BR" sz="2000"/>
+                      <a:rPr lang="mr-IN" sz="2000"/>
                       <a:pPr/>
                       <a:t>[PERCENTUALE]</a:t>
                     </a:fld>
@@ -8322,6 +8356,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8329,13 +8364,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
                     <a:fld id="{E3623109-11E4-B446-BF05-B9EC4E702473}" type="PERCENTAGE">
-                      <a:rPr lang="pt-BR" sz="2000"/>
+                      <a:rPr lang="mr-IN" sz="2000"/>
                       <a:pPr/>
                       <a:t>[PERCENTUALE]</a:t>
                     </a:fld>
@@ -8352,6 +8388,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8359,13 +8396,14 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
                     <a:fld id="{3BD17368-7DD1-C94A-A6A8-C61C9501941E}" type="PERCENTAGE">
-                      <a:rPr lang="pt-BR" sz="2000"/>
+                      <a:rPr lang="mr-IN" sz="2000"/>
                       <a:pPr/>
                       <a:t>[PERCENTUALE]</a:t>
                     </a:fld>
@@ -8382,6 +8420,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8602,6 +8641,7 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -8954,7 +8994,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8973,7 +9015,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8992,7 +9036,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9011,7 +9057,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9030,7 +9078,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9100,7 +9150,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9148,10 +9200,10 @@
                   <c:v>218.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>267.0</c:v>
+                  <c:v>281.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9203,6 +9255,7 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -9555,7 +9608,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9574,7 +9629,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9593,7 +9650,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9663,7 +9722,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9766,6 +9827,7 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -10370,11 +10432,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2144485888"/>
-        <c:axId val="-2144482320"/>
+        <c:axId val="2136540544"/>
+        <c:axId val="2136544112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144485888"/>
+        <c:axId val="2136540544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10417,7 +10479,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144482320"/>
+        <c:crossAx val="2136544112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10425,7 +10487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144482320"/>
+        <c:axId val="2136544112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10476,7 +10538,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144485888"/>
+        <c:crossAx val="2136540544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10490,6 +10552,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10854,7 +10917,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -10945,6 +11010,7 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -11608,11 +11674,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2146368752"/>
-        <c:axId val="-2146372304"/>
+        <c:axId val="2133755952"/>
+        <c:axId val="2133759488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146368752"/>
+        <c:axId val="2133755952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11655,7 +11721,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2146372304"/>
+        <c:crossAx val="2133759488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11663,7 +11729,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146372304"/>
+        <c:axId val="2133759488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11714,7 +11780,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2146368752"/>
+        <c:crossAx val="2133755952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12050,11 +12116,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="2123444112"/>
-        <c:axId val="2123440464"/>
+        <c:axId val="2134800240"/>
+        <c:axId val="2134803872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123444112"/>
+        <c:axId val="2134800240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12092,7 +12158,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123440464"/>
+        <c:crossAx val="2134803872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12100,7 +12166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123440464"/>
+        <c:axId val="2134803872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12163,7 +12229,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123444112"/>
+        <c:crossAx val="2134800240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12741,11 +12807,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2145019184"/>
-        <c:axId val="-2145015648"/>
+        <c:axId val="2133921072"/>
+        <c:axId val="2133917520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2145019184"/>
+        <c:axId val="2133921072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12788,7 +12854,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145015648"/>
+        <c:crossAx val="2133917520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12796,7 +12862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145015648"/>
+        <c:axId val="2133917520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12847,7 +12913,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145019184"/>
+        <c:crossAx val="2133921072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13881,11 +13947,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2123471856"/>
-        <c:axId val="2123435056"/>
+        <c:axId val="2135031936"/>
+        <c:axId val="2135035472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123471856"/>
+        <c:axId val="2135031936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13928,7 +13994,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123435056"/>
+        <c:crossAx val="2135035472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13936,7 +14002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123435056"/>
+        <c:axId val="2135035472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13987,7 +14053,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123471856"/>
+        <c:crossAx val="2135031936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -31454,8 +31520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A71" zoomScale="83" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView showRuler="0" zoomScale="83" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31709,52 +31775,52 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
@@ -31762,81 +31828,81 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="7">
         <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9"/>
-      <c r="B84" s="8"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="7"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="7">
         <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="9"/>
-      <c r="B86" s="8"/>
+      <c r="A86" s="8"/>
+      <c r="B86" s="7"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="9" t="s">
+      <c r="A87" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="8">
+      <c r="B87" s="7">
         <v>750</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9"/>
-      <c r="B88" s="8"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="7"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="8">
+      <c r="B89" s="7">
         <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="9"/>
-      <c r="B90" s="8"/>
+      <c r="A90" s="8"/>
+      <c r="B90" s="7"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="7"/>
-      <c r="B91" s="8"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="7"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="7"/>
-      <c r="B92" s="8"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32159,52 +32225,52 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7">
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="7">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -32481,103 +32547,111 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B80" s="7">
         <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="9"/>
-      <c r="B81" s="8"/>
+      <c r="A81" s="8"/>
+      <c r="B81" s="7"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B82" s="7">
         <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="9"/>
-      <c r="B83" s="8"/>
+      <c r="A83" s="8"/>
+      <c r="B83" s="7"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B84" s="8">
+      <c r="B84" s="7">
         <v>2640</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9"/>
-      <c r="B85" s="8"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="7"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="7">
         <v>975</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="9"/>
-      <c r="B87" s="8"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A43:A44"/>
@@ -32586,14 +32660,6 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32859,103 +32925,111 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="7">
         <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="7">
         <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="9"/>
-      <c r="B87" s="8"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="7"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B88" s="7">
         <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="9"/>
-      <c r="B89" s="8"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="7"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B90" s="8">
+      <c r="B90" s="7">
         <v>1430</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="9"/>
-      <c r="B91" s="8"/>
+      <c r="A91" s="8"/>
+      <c r="B91" s="7"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="8">
+      <c r="B92" s="7">
         <v>630</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="9"/>
-      <c r="B93" s="8"/>
+      <c r="A93" s="8"/>
+      <c r="B93" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="A49:A50"/>
@@ -32964,14 +33038,6 @@
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32982,8 +33048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView showRuler="0" topLeftCell="A69" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33034,14 +33100,14 @@
         <v>10</v>
       </c>
       <c r="F2" s="4">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G2" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2" s="4">
         <f>SUM(B2:G2)</f>
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -33061,14 +33127,14 @@
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G3" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)</f>
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -33088,14 +33154,14 @@
         <v>11</v>
       </c>
       <c r="F4" s="4">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G4" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -33115,14 +33181,14 @@
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G5" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -33142,14 +33208,14 @@
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G6" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -33169,14 +33235,14 @@
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G7" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -33196,14 +33262,14 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -33225,15 +33291,15 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>252</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -33250,160 +33316,174 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="8">
-        <v>137</v>
+      <c r="B49" s="7">
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="8">
-        <v>77</v>
+      <c r="B51" s="7">
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
+      <c r="A77" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="7">
         <v>330</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
-      <c r="B78" s="8"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="7"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
+      <c r="A79" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="7">
         <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="9"/>
-      <c r="B80" s="8"/>
+      <c r="A80" s="8"/>
+      <c r="B80" s="7"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B81" s="7">
         <v>462</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="9"/>
-      <c r="B82" s="8"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="7"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="7">
         <v>2055</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9"/>
-      <c r="B84" s="8"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="7"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="7">
         <f>1155</f>
         <v>1155</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="9"/>
-      <c r="B86" s="8"/>
+      <c r="A86" s="8"/>
+      <c r="B86" s="7"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="8">
+      <c r="B97" s="7">
         <v>210</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="8"/>
+      <c r="B98" s="7"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="8">
+      <c r="B99" s="7">
         <v>140</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="8"/>
+      <c r="B100" s="7"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="8">
+      <c r="B101" s="7">
         <v>1430</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="8"/>
+      <c r="B102" s="7"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="8">
+      <c r="B103" s="7">
         <v>630</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="8"/>
+      <c r="B104" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A51:A52"/>
@@ -33414,20 +33494,6 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33438,8 +33504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showRuler="0" topLeftCell="I1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33487,14 +33553,14 @@
         <v>15</v>
       </c>
       <c r="F2" s="4">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G2" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4">
         <f>SUM(B2:G2)</f>
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -33514,14 +33580,14 @@
         <v>9</v>
       </c>
       <c r="F3" s="4">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G3" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -33541,14 +33607,14 @@
         <v>16</v>
       </c>
       <c r="F4" s="4">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G4" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -33568,14 +33634,14 @@
         <v>14</v>
       </c>
       <c r="F5" s="4">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G5" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -33595,14 +33661,14 @@
         <v>7</v>
       </c>
       <c r="F6" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G6" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -33622,14 +33688,14 @@
         <v>10</v>
       </c>
       <c r="F7" s="4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G7" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -33649,14 +33715,14 @@
         <v>15</v>
       </c>
       <c r="F8" s="4">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -33678,15 +33744,15 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>373</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -33698,139 +33764,127 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="7">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="8">
-        <v>137</v>
+      <c r="B25" s="7">
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="8">
-        <v>119</v>
+      <c r="B27" s="7">
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="7">
         <v>540</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7">
         <v>1892</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="7"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>2055</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <v>1785</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -33839,6 +33893,18 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -34161,131 +34227,141 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="12">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="11"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="12"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="8">
+      <c r="B75" s="7">
         <v>420</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="8"/>
+      <c r="B76" s="7"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
+      <c r="A77" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="7">
         <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
-      <c r="B78" s="8"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="7"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
+      <c r="A79" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="7">
         <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="9"/>
-      <c r="B80" s="8"/>
+      <c r="A80" s="8"/>
+      <c r="B80" s="7"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B81" s="7">
         <v>1035</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="9"/>
-      <c r="B82" s="8"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="7"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B83" s="11">
+      <c r="B83" s="12">
         <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9"/>
-      <c r="B84" s="11"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="12"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="10"/>
+      <c r="A86" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B81:B82"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -34296,16 +34372,6 @@
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B81:B82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -34315,157 +34381,157 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K109"/>
+  <dimension ref="A3:L109"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E86" workbookViewId="0">
+      <selection activeCell="L111" sqref="L111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8">
-        <v>148</v>
+      <c r="B11" s="7">
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8">
-        <v>267</v>
+      <c r="B13" s="7">
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <v>1230</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>620</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>750</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="9"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="7">
         <v>4796</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="9"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="7">
         <v>2220</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="7">
         <v>4005</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -34652,39 +34718,39 @@
       </c>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E94" s="15" t="s">
+      <c r="E94" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F94" s="15" t="s">
+      <c r="F94" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G94" s="15" t="s">
+      <c r="G94" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H94" s="15" t="s">
+      <c r="H94" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I94" s="15" t="s">
+      <c r="I94" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="J94" s="15" t="s">
+      <c r="J94" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="K94" s="15" t="s">
+      <c r="K94" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E95" s="15"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
-      <c r="I95" s="15"/>
-      <c r="J95" s="15"/>
-      <c r="K95" s="15"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16"/>
     </row>
     <row r="96" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E96" s="16" t="s">
+      <c r="E96" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F96" s="14">
@@ -34706,17 +34772,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E97" s="16"/>
+    <row r="97" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E97" s="17"/>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
       <c r="K97" s="14"/>
+      <c r="L97">
+        <f>SUM(F96:K97)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="98" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E98" s="17" t="s">
+    <row r="98" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E98" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F98" s="14">
@@ -34738,17 +34808,21 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E99" s="17"/>
+    <row r="99" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E99" s="15"/>
       <c r="F99" s="14"/>
       <c r="G99" s="14"/>
       <c r="H99" s="14"/>
       <c r="I99" s="14"/>
       <c r="J99" s="14"/>
       <c r="K99" s="14"/>
+      <c r="L99">
+        <f>SUM(F98:K99)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="100" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E100" s="17" t="s">
+    <row r="100" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E100" s="15" t="s">
         <v>25</v>
       </c>
       <c r="F100" s="14">
@@ -34770,17 +34844,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="101" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E101" s="17"/>
+    <row r="101" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E101" s="15"/>
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
       <c r="K101" s="14"/>
+      <c r="L101">
+        <f>SUM(F100:K101)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="102" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E102" s="17" t="s">
+    <row r="102" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E102" s="15" t="s">
         <v>26</v>
       </c>
       <c r="F102" s="14">
@@ -34802,17 +34880,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E103" s="17"/>
+    <row r="103" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E103" s="15"/>
       <c r="F103" s="14"/>
       <c r="G103" s="14"/>
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
       <c r="K103" s="14"/>
+      <c r="L103">
+        <f>SUM(F102:K103)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="104" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E104" s="17" t="s">
+    <row r="104" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E104" s="15" t="s">
         <v>27</v>
       </c>
       <c r="F104" s="14">
@@ -34834,17 +34916,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E105" s="17"/>
+    <row r="105" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E105" s="15"/>
       <c r="F105" s="14"/>
       <c r="G105" s="14"/>
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="14"/>
       <c r="K105" s="14"/>
+      <c r="L105">
+        <f>SUM(F104:K105)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="106" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E106" s="17" t="s">
+    <row r="106" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E106" s="15" t="s">
         <v>28</v>
       </c>
       <c r="F106" s="14">
@@ -34866,17 +34952,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E107" s="17"/>
+    <row r="107" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E107" s="15"/>
       <c r="F107" s="14"/>
       <c r="G107" s="14"/>
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="14"/>
       <c r="K107" s="14"/>
+      <c r="L107">
+        <f>SUM(F106:K107)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="108" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E108" s="17" t="s">
+    <row r="108" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E108" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F108" s="14">
@@ -34898,59 +34988,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E109" s="17"/>
+    <row r="109" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E109" s="15"/>
       <c r="F109" s="14"/>
       <c r="G109" s="14"/>
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
       <c r="J109" s="14"/>
       <c r="K109" s="14"/>
+      <c r="L109">
+        <f>SUM(F108:K109)</f>
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="K102:K103"/>
-    <mergeCell ref="J100:J101"/>
-    <mergeCell ref="K100:K101"/>
-    <mergeCell ref="J98:J99"/>
-    <mergeCell ref="K98:K99"/>
-    <mergeCell ref="J108:J109"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="J106:J107"/>
-    <mergeCell ref="K106:K107"/>
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="K104:K105"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="I108:I109"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="G106:G107"/>
-    <mergeCell ref="H106:H107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="H104:H105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="F102:F103"/>
-    <mergeCell ref="G102:G103"/>
-    <mergeCell ref="H102:H103"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="G100:G101"/>
-    <mergeCell ref="H100:H101"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="G98:G99"/>
-    <mergeCell ref="H98:H99"/>
-    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="J96:J97"/>
     <mergeCell ref="K96:K97"/>
     <mergeCell ref="H94:H95"/>
@@ -34965,30 +35041,48 @@
     <mergeCell ref="J94:J95"/>
     <mergeCell ref="K94:K95"/>
     <mergeCell ref="I96:I97"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="G98:G99"/>
+    <mergeCell ref="H98:H99"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="G100:G101"/>
+    <mergeCell ref="H100:H101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="G102:G103"/>
+    <mergeCell ref="H102:H103"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="G106:G107"/>
+    <mergeCell ref="H106:H107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="I108:I109"/>
+    <mergeCell ref="J108:J109"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="J106:J107"/>
+    <mergeCell ref="K106:K107"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="K104:K105"/>
+    <mergeCell ref="J102:J103"/>
+    <mergeCell ref="K102:K103"/>
+    <mergeCell ref="J100:J101"/>
+    <mergeCell ref="K100:K101"/>
+    <mergeCell ref="J98:J99"/>
+    <mergeCell ref="K98:K99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[PdP] - Corretti dati tabelle sezioni 5 e 6. Stesura Consuntivo di Periodo comprensivo di ri-pianificazione per rientrare nei costi completata. Analisi dei rischi aggiornata. Diario aggiornato.
</commit_message>
<xml_diff>
--- a/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13880" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ARM" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="PDCOD" sheetId="9" r:id="rId7"/>
     <sheet name="VV" sheetId="6" r:id="rId8"/>
     <sheet name="Tot" sheetId="7" r:id="rId9"/>
+    <sheet name="Foglio1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -134,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +194,22 @@
       <color theme="1"/>
       <name val="TeXGyreHeros"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="TeXGyreHeros"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="TeXGyreHeros"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -256,19 +273,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -823,11 +851,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2134747456"/>
-        <c:axId val="2134751008"/>
+        <c:axId val="2107255024"/>
+        <c:axId val="2107228192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134747456"/>
+        <c:axId val="2107255024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +898,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134751008"/>
+        <c:crossAx val="2107228192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -878,7 +906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134751008"/>
+        <c:axId val="2107228192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +957,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134747456"/>
+        <c:crossAx val="2107255024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,7 +971,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1972,11 +1999,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2104320208"/>
-        <c:axId val="2104323744"/>
+        <c:axId val="2108643728"/>
+        <c:axId val="2108647264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104320208"/>
+        <c:axId val="2108643728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2019,7 +2046,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104323744"/>
+        <c:crossAx val="2108647264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2027,7 +2054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104323744"/>
+        <c:axId val="2108647264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,7 +2105,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104320208"/>
+        <c:crossAx val="2108643728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3445,7 +3472,7 @@
                   <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>22.0</c:v>
@@ -3457,7 +3484,7 @@
                   <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3529,7 +3556,7 @@
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>24.0</c:v>
@@ -3541,7 +3568,7 @@
                   <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3557,11 +3584,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2136063280"/>
-        <c:axId val="2136066816"/>
+        <c:axId val="2106396704"/>
+        <c:axId val="2106400240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2136063280"/>
+        <c:axId val="2106396704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3604,7 +3631,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136066816"/>
+        <c:crossAx val="2106400240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3612,7 +3639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136066816"/>
+        <c:axId val="2106400240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3663,7 +3690,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136063280"/>
+        <c:crossAx val="2106396704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3677,7 +3704,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3998,17 +4024,15 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0517523467461305"/>
-                  <c:y val="0.104367750946299"/>
+                  <c:x val="-0.0403322245052505"/>
+                  <c:y val="0.0852005687495979"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -4019,9 +4043,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4040,9 +4062,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4112,9 +4132,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4147,19 +4165,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>193.0</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>91.0</c:v>
+                  <c:v>97.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4207,7 +4225,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -4520,9 +4537,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4541,9 +4556,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4613,9 +4626,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4648,19 +4659,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>330.0</c:v>
+                  <c:v>390.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>462.0</c:v>
+                  <c:v>924.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2055.0</c:v>
+                  <c:v>2160.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1155.0</c:v>
+                  <c:v>1245.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4708,7 +4719,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5201,7 +5211,7 @@
                   <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>22.0</c:v>
@@ -5213,7 +5223,7 @@
                   <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5279,13 +5289,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>24.0</c:v>
@@ -5297,7 +5307,7 @@
                   <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5313,11 +5323,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2104420048"/>
-        <c:axId val="2104423584"/>
+        <c:axId val="2109816096"/>
+        <c:axId val="2109819632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104420048"/>
+        <c:axId val="2109816096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5360,7 +5370,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104423584"/>
+        <c:crossAx val="2109819632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5368,7 +5378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104423584"/>
+        <c:axId val="2109819632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5419,7 +5429,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104420048"/>
+        <c:crossAx val="2109816096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5433,7 +5443,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5733,9 +5742,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5805,9 +5812,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5840,19 +5845,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>18.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86.0</c:v>
+                  <c:v>107.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>193.0</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>133.0</c:v>
+                  <c:v>139.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5900,7 +5905,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6203,9 +6207,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6275,9 +6277,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6310,19 +6310,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>540.0</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260.0</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1892.0</c:v>
+                  <c:v>2354.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2055.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1785.0</c:v>
+                  <c:v>2085.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6370,7 +6370,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6707,9 +6706,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6792,7 +6789,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -7397,11 +7393,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2104452928"/>
-        <c:axId val="2104456464"/>
+        <c:axId val="2109767440"/>
+        <c:axId val="2109833568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2104452928"/>
+        <c:axId val="2109767440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7444,7 +7440,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104456464"/>
+        <c:crossAx val="2109833568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7452,7 +7448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104456464"/>
+        <c:axId val="2109833568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7503,7 +7499,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104452928"/>
+        <c:crossAx val="2109767440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7517,6 +7513,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7940,19 +7937,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>14.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>69.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8300,7 +8297,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8324,7 +8320,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8332,7 +8327,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.109240159365692"/>
+                  <c:y val="0.0458165109506451"/>
+                </c:manualLayout>
+              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8347,7 +8347,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:dLblPos val="ctr"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8356,7 +8356,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8364,7 +8363,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8388,7 +8386,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8396,7 +8393,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8420,7 +8416,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8581,19 +8576,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>420.0</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160.0</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>264.0</c:v>
+                  <c:v>132.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1035.0</c:v>
+                  <c:v>795.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165.0</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8641,7 +8636,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -8982,8 +8976,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.043000656167979"/>
-                  <c:y val="0.0838101487314086"/>
+                  <c:x val="-0.0266607482888168"/>
+                  <c:y val="0.0715190191933973"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -8994,17 +8988,15 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.126665791776028"/>
-                  <c:y val="0.250382400116652"/>
+                  <c:x val="-0.0939860274818589"/>
+                  <c:y val="0.24546605346898"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -9015,17 +9007,15 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.110312992125984"/>
-                  <c:y val="0.109202391367746"/>
+                  <c:x val="-0.0596594359528588"/>
+                  <c:y val="0.101827785907293"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -9036,9 +9026,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9057,9 +9045,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9078,9 +9064,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9150,9 +9134,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9188,22 +9170,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>41.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>218.0</c:v>
+                  <c:v>233.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>204.0</c:v>
+                  <c:v>208.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>281.0</c:v>
+                  <c:v>257.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9255,7 +9237,6 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -9608,9 +9589,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9629,9 +9608,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9650,9 +9627,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9722,9 +9697,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9760,22 +9733,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1230.0</c:v>
+                  <c:v>1110.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>620.0</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>750.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4796.0</c:v>
+                  <c:v>5126.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2220.0</c:v>
+                  <c:v>2280.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4005.0</c:v>
+                  <c:v>3855.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9827,7 +9800,6 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -9978,7 +9950,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.0</c:v>
@@ -10398,7 +10370,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>33.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>46.0</c:v>
@@ -10432,11 +10404,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2136540544"/>
-        <c:axId val="2136544112"/>
+        <c:axId val="2107554800"/>
+        <c:axId val="2106522480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2136540544"/>
+        <c:axId val="2107554800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10479,7 +10451,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136544112"/>
+        <c:crossAx val="2106522480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10487,7 +10459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136544112"/>
+        <c:axId val="2106522480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10538,7 +10510,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136540544"/>
+        <c:crossAx val="2107554800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10552,7 +10524,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10917,9 +10888,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11010,7 +10979,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -11674,11 +11642,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2133755952"/>
-        <c:axId val="2133759488"/>
+        <c:axId val="2109136176"/>
+        <c:axId val="2109139712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2133755952"/>
+        <c:axId val="2109136176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11721,7 +11689,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133759488"/>
+        <c:crossAx val="2109139712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11729,7 +11697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133759488"/>
+        <c:axId val="2109139712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11780,7 +11748,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133755952"/>
+        <c:crossAx val="2109136176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12116,11 +12084,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="2134800240"/>
-        <c:axId val="2134803872"/>
+        <c:axId val="2108480672"/>
+        <c:axId val="2108534368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134800240"/>
+        <c:axId val="2108480672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12158,7 +12126,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134803872"/>
+        <c:crossAx val="2108534368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12166,7 +12134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134803872"/>
+        <c:axId val="2108534368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12229,7 +12197,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134800240"/>
+        <c:crossAx val="2108480672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12807,11 +12775,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2133921072"/>
-        <c:axId val="2133917520"/>
+        <c:axId val="2106239536"/>
+        <c:axId val="2106243072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2133921072"/>
+        <c:axId val="2106239536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12854,7 +12822,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133917520"/>
+        <c:crossAx val="2106243072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12862,7 +12830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133917520"/>
+        <c:axId val="2106243072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12913,7 +12881,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133921072"/>
+        <c:crossAx val="2106239536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13947,11 +13915,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2135031936"/>
-        <c:axId val="2135035472"/>
+        <c:axId val="2106290576"/>
+        <c:axId val="2106294112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135031936"/>
+        <c:axId val="2106290576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13994,7 +13962,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135035472"/>
+        <c:crossAx val="2106294112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14002,7 +13970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135035472"/>
+        <c:axId val="2106294112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14053,7 +14021,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135031936"/>
+        <c:crossAx val="2106290576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -31521,7 +31489,7 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="83" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31775,52 +31743,52 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="10">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="10">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="10">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
@@ -31828,84 +31796,246 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="10">
         <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="7"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="10"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="10">
         <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="7"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="10"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B87" s="10">
         <v>750</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="8"/>
-      <c r="B88" s="7"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="10"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="8" t="s">
+      <c r="A89" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="10">
         <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="7"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="10"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="9"/>
-      <c r="B91" s="7"/>
+      <c r="B91" s="10"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="9"/>
-      <c r="B92" s="7"/>
+      <c r="B92" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A91:A92"/>
     <mergeCell ref="B91:B92"/>
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="B87:B88"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7">
+        <v>28</v>
+      </c>
+      <c r="C1" s="8">
+        <v>17</v>
+      </c>
+      <c r="D1" s="8">
+        <v>47</v>
+      </c>
+      <c r="E1">
+        <v>16</v>
+      </c>
+      <c r="F1">
+        <f t="shared" ref="F1:F7" si="0">SUM(A1:E1)</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7">
+        <v>28</v>
+      </c>
+      <c r="C2" s="8">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8">
+        <v>46</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7">
+        <v>29</v>
+      </c>
+      <c r="C5" s="8">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7">
+        <v>28</v>
+      </c>
+      <c r="C6" s="8">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -31970,8 +32100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A43" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView showRuler="0" zoomScale="178" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32225,52 +32355,52 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="10">
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -32292,8 +32422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A76" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showRuler="0" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32547,103 +32677,111 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="10">
         <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="10">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80" s="10">
         <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="8"/>
-      <c r="B81" s="7"/>
+      <c r="A81" s="11"/>
+      <c r="B81" s="10"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="7">
+      <c r="B82" s="10">
         <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
-      <c r="B83" s="7"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="10"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84" s="10">
         <v>2640</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8"/>
-      <c r="B85" s="7"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="10"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86" s="10">
         <v>975</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="7"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="B84:B85"/>
     <mergeCell ref="A86:A87"/>
@@ -32652,14 +32790,6 @@
     <mergeCell ref="B80:B81"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32671,7 +32801,7 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="124" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32925,103 +33055,111 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="10">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="10">
         <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86" s="10">
         <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="7"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="10"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B88" s="10">
         <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="8"/>
-      <c r="B89" s="7"/>
+      <c r="A89" s="11"/>
+      <c r="B89" s="10"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B90" s="7">
+      <c r="B90" s="10">
         <v>1430</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="8"/>
-      <c r="B91" s="7"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="10"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="8" t="s">
+      <c r="A92" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B92" s="10">
         <v>630</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="8"/>
-      <c r="B93" s="7"/>
+      <c r="A93" s="11"/>
+      <c r="B93" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A90:A91"/>
     <mergeCell ref="B90:B91"/>
     <mergeCell ref="A92:A93"/>
@@ -33030,14 +33168,6 @@
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B88:B89"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33048,8 +33178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A69" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView showRuler="0" topLeftCell="A40" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33154,10 +33284,10 @@
         <v>11</v>
       </c>
       <c r="F4" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
@@ -33262,10 +33392,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
@@ -33316,174 +33446,161 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="7">
-        <v>11</v>
+      <c r="B43" s="10">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="7">
-        <v>6</v>
+      <c r="B45" s="10">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="7">
-        <v>21</v>
+      <c r="B47" s="10">
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="7">
-        <v>193</v>
+      <c r="B49" s="10">
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="7">
-        <v>91</v>
+      <c r="B51" s="10">
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="7">
-        <v>330</v>
+      <c r="B77" s="10">
+        <v>390</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="10"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="7">
-        <v>120</v>
+      <c r="B79" s="10">
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="7"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="10"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="7">
-        <v>462</v>
+      <c r="B81" s="10">
+        <f>462*2</f>
+        <v>924</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="7"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="10"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="7">
-        <v>2055</v>
+      <c r="B83" s="10">
+        <v>2160</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="7"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="10"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="7">
-        <f>1155</f>
-        <v>1155</v>
+      <c r="B85" s="10">
+        <f>1155+90</f>
+        <v>1245</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="7"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="10"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="7">
+      <c r="B97" s="10">
         <v>210</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="7"/>
+      <c r="B98" s="10"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="7">
+      <c r="B99" s="10">
         <v>140</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="7"/>
+      <c r="B100" s="10"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="7">
+      <c r="B101" s="10">
         <v>1430</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="7"/>
+      <c r="B102" s="10"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="7">
+      <c r="B103" s="10">
         <v>630</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="7"/>
+      <c r="B104" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A51:A52"/>
@@ -33494,6 +33611,20 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33504,11 +33635,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="I1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showRuler="0" zoomScale="138" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -33556,11 +33690,11 @@
         <v>30</v>
       </c>
       <c r="G2" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4">
         <f>SUM(B2:G2)</f>
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -33607,10 +33741,10 @@
         <v>16</v>
       </c>
       <c r="F4" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
@@ -33715,10 +33849,10 @@
         <v>15</v>
       </c>
       <c r="F8" s="4">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
@@ -33748,11 +33882,11 @@
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -33764,127 +33898,139 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="7">
-        <v>18</v>
+      <c r="B19" s="10">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="7">
-        <v>13</v>
+      <c r="B21" s="10">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="7">
-        <v>86</v>
+      <c r="B23" s="10">
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="7">
-        <v>193</v>
+      <c r="B25" s="10">
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="7">
-        <v>133</v>
+      <c r="B27" s="10">
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="7">
-        <v>540</v>
+      <c r="B36" s="10">
+        <v>600</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="7">
-        <v>260</v>
+      <c r="B38" s="10">
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="7">
-        <v>1892</v>
+      <c r="B40" s="10">
+        <v>2354</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="7">
-        <v>2055</v>
+      <c r="B42" s="10">
+        <v>3000</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="10"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="7">
-        <v>1785</v>
+      <c r="B44" s="10">
+        <v>2085</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -33893,18 +34039,6 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -33915,8 +34049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A71" zoomScale="113" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="113" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34145,7 +34279,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f>SUM(C2:C8)</f>
         <v>8</v>
       </c>
       <c r="D9">
@@ -34227,131 +34361,141 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="7">
-        <v>14</v>
+      <c r="B38" s="10">
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="7">
-        <v>8</v>
+      <c r="B40" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="7">
-        <v>12</v>
+      <c r="B42" s="10">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="7">
-        <v>11</v>
+      <c r="B44" s="10">
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="10"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="12">
-        <v>69</v>
+      <c r="B46" s="13">
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="7">
-        <v>420</v>
+      <c r="B75" s="10">
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
+      <c r="B76" s="10"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="7">
-        <v>160</v>
+      <c r="B77" s="10">
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="10"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="7">
-        <v>264</v>
+      <c r="B79" s="10">
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="7"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="10"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="7">
-        <v>1035</v>
+      <c r="B81" s="10">
+        <v>795</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="7"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="10"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B83" s="12">
-        <v>165</v>
+      <c r="B83" s="13">
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="12"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="13"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="13"/>
+      <c r="A86" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B46:B47"/>
     <mergeCell ref="A77:A78"/>
     <mergeCell ref="B75:B76"/>
     <mergeCell ref="A79:A80"/>
@@ -34362,16 +34506,6 @@
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="A83:A84"/>
     <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -34383,155 +34517,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E86" workbookViewId="0">
-      <selection activeCell="L111" sqref="L111"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K96" sqref="K96:K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7">
-        <v>41</v>
+      <c r="B3" s="10">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7">
-        <v>31</v>
+      <c r="B5" s="10">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="10">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="7">
-        <v>218</v>
+      <c r="B9" s="10">
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7">
-        <v>204</v>
+      <c r="B11" s="10">
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7">
-        <v>281</v>
+      <c r="B13" s="10">
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="7">
-        <v>1230</v>
+      <c r="B43" s="10">
+        <v>1110</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="10"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="7">
-        <v>620</v>
+      <c r="B45" s="10">
+        <v>500</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="10"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="10">
         <v>750</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="7">
-        <v>4796</v>
+      <c r="B49" s="10">
+        <v>5126</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="8"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="7">
-        <v>2220</v>
+      <c r="B51" s="10">
+        <v>2280</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="10"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="7">
-        <v>4005</v>
+      <c r="B53" s="10">
+        <v>3855</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="10"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -34718,284 +34852,284 @@
       </c>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F94" s="16" t="s">
+      <c r="F94" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G94" s="16" t="s">
+      <c r="G94" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H94" s="16" t="s">
+      <c r="H94" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I94" s="16" t="s">
+      <c r="I94" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J94" s="16" t="s">
+      <c r="J94" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K94" s="16" t="s">
+      <c r="K94" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E95" s="16"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
-      <c r="J95" s="16"/>
-      <c r="K95" s="16"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="20"/>
     </row>
     <row r="96" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E96" s="17" t="s">
+      <c r="E96" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F96" s="14">
-        <v>9</v>
-      </c>
-      <c r="G96" s="14">
+      <c r="F96" s="16">
+        <v>10</v>
+      </c>
+      <c r="G96" s="16">
         <v>0</v>
       </c>
-      <c r="H96" s="14">
+      <c r="H96" s="16">
         <v>6</v>
       </c>
-      <c r="I96" s="14">
+      <c r="I96" s="16">
         <v>35</v>
       </c>
-      <c r="J96" s="14">
+      <c r="J96" s="16">
         <v>22</v>
       </c>
-      <c r="K96" s="14">
-        <v>33</v>
+      <c r="K96" s="17">
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E97" s="17"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
-      <c r="H97" s="14"/>
-      <c r="I97" s="14"/>
-      <c r="J97" s="14"/>
-      <c r="K97" s="14"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
+      <c r="J97" s="16"/>
+      <c r="K97" s="17"/>
       <c r="L97">
         <f>SUM(F96:K97)</f>
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="98" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E98" s="15" t="s">
+      <c r="E98" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F98" s="14">
+      <c r="F98" s="16">
         <v>7</v>
       </c>
-      <c r="G98" s="14">
+      <c r="G98" s="16">
         <v>3</v>
       </c>
-      <c r="H98" s="14">
+      <c r="H98" s="16">
         <v>6</v>
       </c>
-      <c r="I98" s="14">
+      <c r="I98" s="16">
         <v>27</v>
       </c>
-      <c r="J98" s="14">
+      <c r="J98" s="16">
         <v>16</v>
       </c>
-      <c r="K98" s="14">
+      <c r="K98" s="22">
         <v>46</v>
       </c>
     </row>
     <row r="99" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E99" s="15"/>
-      <c r="F99" s="14"/>
-      <c r="G99" s="14"/>
-      <c r="H99" s="14"/>
-      <c r="I99" s="14"/>
-      <c r="J99" s="14"/>
-      <c r="K99" s="14"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="16"/>
+      <c r="I99" s="16"/>
+      <c r="J99" s="16"/>
+      <c r="K99" s="22"/>
       <c r="L99">
         <f>SUM(F98:K99)</f>
         <v>105</v>
       </c>
     </row>
     <row r="100" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E100" s="15" t="s">
+      <c r="E100" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F100" s="14">
+      <c r="F100" s="16">
         <v>4</v>
       </c>
-      <c r="G100" s="14">
+      <c r="G100" s="16">
         <v>11</v>
       </c>
-      <c r="H100" s="14">
+      <c r="H100" s="16">
         <v>0</v>
       </c>
-      <c r="I100" s="14">
+      <c r="I100" s="16">
         <v>31</v>
       </c>
-      <c r="J100" s="14">
+      <c r="J100" s="16">
         <v>19</v>
       </c>
-      <c r="K100" s="14">
+      <c r="K100" s="22">
         <v>40</v>
       </c>
     </row>
     <row r="101" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E101" s="15"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14"/>
-      <c r="J101" s="14"/>
-      <c r="K101" s="14"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
+      <c r="J101" s="16"/>
+      <c r="K101" s="22"/>
       <c r="L101">
         <f>SUM(F100:K101)</f>
         <v>105</v>
       </c>
     </row>
     <row r="102" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E102" s="15" t="s">
+      <c r="E102" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F102" s="14">
+      <c r="F102" s="16">
         <v>4</v>
       </c>
-      <c r="G102" s="14">
+      <c r="G102" s="16">
         <v>5</v>
       </c>
-      <c r="H102" s="14">
+      <c r="H102" s="16">
         <v>7</v>
       </c>
-      <c r="I102" s="14">
+      <c r="I102" s="16">
         <v>40</v>
       </c>
-      <c r="J102" s="14">
+      <c r="J102" s="16">
         <v>17</v>
       </c>
-      <c r="K102" s="14">
+      <c r="K102" s="22">
         <v>32</v>
       </c>
     </row>
     <row r="103" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E103" s="15"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="14"/>
-      <c r="K103" s="14"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
+      <c r="K103" s="22"/>
       <c r="L103">
         <f>SUM(F102:K103)</f>
         <v>105</v>
       </c>
     </row>
     <row r="104" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E104" s="15" t="s">
+      <c r="E104" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F104" s="14">
+      <c r="F104" s="16">
         <v>3</v>
       </c>
-      <c r="G104" s="14">
+      <c r="G104" s="16">
         <v>0</v>
       </c>
-      <c r="H104" s="14">
+      <c r="H104" s="16">
         <v>6</v>
       </c>
-      <c r="I104" s="14">
+      <c r="I104" s="16">
         <v>21</v>
       </c>
-      <c r="J104" s="14">
+      <c r="J104" s="16">
         <v>26</v>
       </c>
-      <c r="K104" s="14">
+      <c r="K104" s="22">
         <v>49</v>
       </c>
     </row>
     <row r="105" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E105" s="15"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="14"/>
-      <c r="K105" s="14"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="16"/>
+      <c r="I105" s="16"/>
+      <c r="J105" s="16"/>
+      <c r="K105" s="22"/>
       <c r="L105">
         <f>SUM(F104:K105)</f>
         <v>105</v>
       </c>
     </row>
     <row r="106" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E106" s="15" t="s">
+      <c r="E106" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F106" s="14">
+      <c r="F106" s="16">
         <v>4</v>
       </c>
-      <c r="G106" s="14">
+      <c r="G106" s="16">
         <v>4</v>
       </c>
-      <c r="H106" s="14">
+      <c r="H106" s="16">
         <v>5</v>
       </c>
-      <c r="I106" s="14">
+      <c r="I106" s="16">
         <v>26</v>
       </c>
-      <c r="J106" s="14">
+      <c r="J106" s="16">
         <v>26</v>
       </c>
-      <c r="K106" s="14">
+      <c r="K106" s="22">
         <v>40</v>
       </c>
     </row>
     <row r="107" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E107" s="15"/>
-      <c r="F107" s="14"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="14"/>
-      <c r="J107" s="14"/>
-      <c r="K107" s="14"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="16"/>
+      <c r="K107" s="22"/>
       <c r="L107">
         <f>SUM(F106:K107)</f>
         <v>105</v>
       </c>
     </row>
     <row r="108" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E108" s="15" t="s">
+      <c r="E108" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F108" s="14">
+      <c r="F108" s="16">
         <v>10</v>
       </c>
-      <c r="G108" s="14">
+      <c r="G108" s="16">
         <v>8</v>
       </c>
-      <c r="H108" s="14">
+      <c r="H108" s="16">
         <v>0</v>
       </c>
-      <c r="I108" s="14">
+      <c r="I108" s="16">
         <v>38</v>
       </c>
-      <c r="J108" s="14">
+      <c r="J108" s="16">
         <v>22</v>
       </c>
-      <c r="K108" s="14">
+      <c r="K108" s="22">
         <v>27</v>
       </c>
     </row>
     <row r="109" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E109" s="15"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14"/>
-      <c r="J109" s="14"/>
-      <c r="K109" s="14"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+      <c r="J109" s="16"/>
+      <c r="K109" s="22"/>
       <c r="L109">
         <f>SUM(F108:K109)</f>
         <v>105</v>
@@ -35003,30 +35137,48 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="J102:J103"/>
+    <mergeCell ref="K102:K103"/>
+    <mergeCell ref="J100:J101"/>
+    <mergeCell ref="K100:K101"/>
+    <mergeCell ref="J98:J99"/>
+    <mergeCell ref="K98:K99"/>
+    <mergeCell ref="J108:J109"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="J106:J107"/>
+    <mergeCell ref="K106:K107"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="K104:K105"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="I108:I109"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="G106:G107"/>
+    <mergeCell ref="H106:H107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="G102:G103"/>
+    <mergeCell ref="H102:H103"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="G100:G101"/>
+    <mergeCell ref="H100:H101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="G98:G99"/>
+    <mergeCell ref="H98:H99"/>
+    <mergeCell ref="I98:I99"/>
     <mergeCell ref="J96:J97"/>
     <mergeCell ref="K96:K97"/>
     <mergeCell ref="H94:H95"/>
@@ -35041,48 +35193,30 @@
     <mergeCell ref="J94:J95"/>
     <mergeCell ref="K94:K95"/>
     <mergeCell ref="I96:I97"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="G98:G99"/>
-    <mergeCell ref="H98:H99"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="G100:G101"/>
-    <mergeCell ref="H100:H101"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="F102:F103"/>
-    <mergeCell ref="G102:G103"/>
-    <mergeCell ref="H102:H103"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="H104:H105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="G106:G107"/>
-    <mergeCell ref="H106:H107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="I108:I109"/>
-    <mergeCell ref="J108:J109"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="J106:J107"/>
-    <mergeCell ref="K106:K107"/>
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="K104:K105"/>
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="K102:K103"/>
-    <mergeCell ref="J100:J101"/>
-    <mergeCell ref="K100:K101"/>
-    <mergeCell ref="J98:J99"/>
-    <mergeCell ref="K98:K99"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>